<commit_message>
Added for AM work
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites-Exp/TRIP700A.xlsx
+++ b/JupyterNotebooks/AveragedIntensites-Exp/TRIP700A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1344,65 +1344,65 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HexGrid-90degTilt5degRes</t>
+          <t>HexGrid-90degTilt22p5degRes</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9925198466865341</v>
+        <v>0.999519819632665</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9923480365276607</v>
+        <v>1.017562233915762</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9912463130490972</v>
+        <v>0.9828356523002032</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9909893856402903</v>
+        <v>0.9922549711631075</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9925198466865341</v>
+        <v>0.999519819632665</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9923480365276607</v>
+        <v>1.017562233915762</v>
       </c>
       <c r="I14" t="n">
-        <v>0.990870661866622</v>
+        <v>0.9834194394324258</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9908381835054233</v>
+        <v>0.9833850312650245</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9905033285288765</v>
+        <v>0.988071276157061</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9904279454116482</v>
+        <v>1.002057048397828</v>
       </c>
       <c r="M14" t="n">
-        <v>0.9925003681086734</v>
+        <v>0.9994806574392824</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9917971747883789</v>
+        <v>1.000198943107983</v>
       </c>
       <c r="O14" t="n">
-        <v>0.9916687110839755</v>
+        <v>1.004908602539435</v>
       </c>
       <c r="P14" t="n">
-        <v>0.9920380654210973</v>
+        <v>0.9999725686162101</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.991527911739016</v>
+        <v>0.9975509524596907</v>
       </c>
       <c r="R14" t="n">
-        <v>0.9920380654210973</v>
+        <v>0.9999725686162101</v>
       </c>
       <c r="S14" t="n">
-        <v>0.9917758954758955</v>
+        <v>0.9980431692529343</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9919246857180232</v>
+        <v>0.9983384993288805</v>
       </c>
       <c r="U14" t="n">
-        <v>0.991217962652019</v>
+        <v>0.9936381840330096</v>
       </c>
     </row>
     <row r="15">
@@ -2006,6 +2006,140 @@
       </c>
       <c r="U23" t="n">
         <v>1.01209683560644</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RotRing Axis-Y Res-5.0 Theta-2.5 </t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1.064566973029285</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.026181214278875</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9493745435035073</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.9960352639173311</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.064566973029285</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.026181214278875</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.9728871906349001</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.9597549947074582</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1.018186068794158</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.993989054773298</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1.064560347927988</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.9877778788911912</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1.011108239098103</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1.013374243603889</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.9905303405665711</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1.013374243603889</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1.00903949868225</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1.020144993551657</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.9976219129548516</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RotRing Axis-Y Res-5.0 Theta-5.0 </t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1.055669658786997</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.016021296484453</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9522480769540386</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.9937391728448696</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.055669658786997</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.016021296484453</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.9768538994046883</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.9639748353499836</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1.012134108143645</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.9933785524706517</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1.055658804731599</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.9841346867192458</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.004880234664661</v>
+      </c>
+      <c r="P25" t="n">
+        <v>1.007979677408496</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.9873361820944537</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1.007979677408496</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1.00441955126759</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1.014669572771471</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.995502450054916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>